<commit_message>
added TruckManager and Greedy classes with many other updates
</commit_message>
<xml_diff>
--- a/data/all_delivery_data.xlsx
+++ b/data/all_delivery_data.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamm\PycharmProjects\TravelingDeliveryman\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADB77642-2E2A-4A4C-9AD7-1CD5920177F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9F50E5-00A9-4F86-81DD-027CE31DC487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4200" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="4200" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="package_data" sheetId="4" r:id="rId1"/>
-    <sheet name="address_table" sheetId="2" r:id="rId2"/>
-    <sheet name="distance_table" sheetId="1" r:id="rId3"/>
-    <sheet name="package_group_table" sheetId="5" r:id="rId4"/>
+    <sheet name="address_data" sheetId="2" r:id="rId2"/>
+    <sheet name="distance_data" sheetId="1" r:id="rId3"/>
+    <sheet name="package_group_data" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">address_table!$A$1:$C$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">address_data!$A$1:$C$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -272,7 +272,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -529,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -581,25 +581,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -882,15 +880,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259C2A56-3C60-479F-941A-D591511CBD81}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="27"/>
+    <col min="3" max="3" width="9.26953125" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="25"/>
     <col min="7" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -901,10 +899,10 @@
       <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="17" t="s">
@@ -916,7 +914,7 @@
       <c r="G1" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="22" t="s">
         <v>71</v>
       </c>
     </row>
@@ -927,10 +925,10 @@
       <c r="B2" s="18">
         <v>5</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="24">
         <v>0.4375</v>
       </c>
       <c r="E2" s="18">
@@ -953,10 +951,10 @@
       <c r="B3" s="18">
         <v>9</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E3" s="18">
@@ -979,10 +977,10 @@
       <c r="B4" s="18">
         <v>8</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E4" s="18">
@@ -1005,10 +1003,10 @@
       <c r="B5" s="18">
         <v>18</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E5" s="18">
@@ -1031,10 +1029,10 @@
       <c r="B6" s="18">
         <v>19</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E6" s="18">
@@ -1057,10 +1055,10 @@
       <c r="B7" s="18">
         <v>13</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="24">
         <v>0.37847222222222227</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="24">
         <v>0.4375</v>
       </c>
       <c r="E7" s="18">
@@ -1083,10 +1081,10 @@
       <c r="B8" s="18">
         <v>2</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E8" s="18">
@@ -1109,10 +1107,10 @@
       <c r="B9" s="18">
         <v>12</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E9" s="18">
@@ -1135,10 +1133,10 @@
       <c r="B10" s="18">
         <v>12</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="24">
         <v>0.43055555555555558</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E10" s="18">
@@ -1161,10 +1159,10 @@
       <c r="B11" s="18">
         <v>25</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E11" s="18">
@@ -1187,10 +1185,10 @@
       <c r="B12" s="18">
         <v>10</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E12" s="18">
@@ -1213,10 +1211,10 @@
       <c r="B13" s="18">
         <v>16</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E13" s="18">
@@ -1239,10 +1237,10 @@
       <c r="B14" s="18">
         <v>6</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="24">
         <v>0.4375</v>
       </c>
       <c r="E14" s="18">
@@ -1265,10 +1263,10 @@
       <c r="B15" s="18">
         <v>20</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="24">
         <v>0.4375</v>
       </c>
       <c r="E15" s="18">
@@ -1291,10 +1289,10 @@
       <c r="B16" s="18">
         <v>21</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="24">
         <v>0.375</v>
       </c>
       <c r="E16" s="18">
@@ -1317,10 +1315,10 @@
       <c r="B17" s="18">
         <v>21</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="24">
         <v>0.4375</v>
       </c>
       <c r="E17" s="18">
@@ -1343,10 +1341,10 @@
       <c r="B18" s="18">
         <v>14</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E18" s="18">
@@ -1369,10 +1367,10 @@
       <c r="B19" s="18">
         <v>3</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E19" s="18">
@@ -1395,10 +1393,10 @@
       <c r="B20" s="18">
         <v>4</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E20" s="18">
@@ -1421,10 +1419,10 @@
       <c r="B21" s="18">
         <v>17</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="24">
         <v>0.4375</v>
       </c>
       <c r="E21" s="18">
@@ -1447,10 +1445,10 @@
       <c r="B22" s="18">
         <v>17</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="D22" s="26">
+      <c r="D22" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E22" s="18">
@@ -1473,10 +1471,10 @@
       <c r="B23" s="18">
         <v>26</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="D23" s="26">
+      <c r="D23" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E23" s="18">
@@ -1499,10 +1497,10 @@
       <c r="B24" s="18">
         <v>23</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C24" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E24" s="18">
@@ -1525,10 +1523,10 @@
       <c r="B25" s="18">
         <v>22</v>
       </c>
-      <c r="C25" s="26">
+      <c r="C25" s="24">
         <v>0.33333333333333298</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E25" s="18">
@@ -1551,10 +1549,10 @@
       <c r="B26" s="18">
         <v>24</v>
       </c>
-      <c r="C26" s="26">
+      <c r="C26" s="24">
         <v>0.37847222222222227</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="24">
         <v>0.4375</v>
       </c>
       <c r="E26" s="18">
@@ -1577,10 +1575,10 @@
       <c r="B27" s="18">
         <v>24</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E27" s="18">
@@ -1603,10 +1601,10 @@
       <c r="B28" s="18">
         <v>1</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D28" s="26">
+      <c r="D28" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E28" s="18">
@@ -1629,10 +1627,10 @@
       <c r="B29" s="18">
         <v>11</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="24">
         <v>0.37847222222222227</v>
       </c>
-      <c r="D29" s="26">
+      <c r="D29" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E29" s="18">
@@ -1655,10 +1653,10 @@
       <c r="B30" s="18">
         <v>2</v>
       </c>
-      <c r="C30" s="26">
+      <c r="C30" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D30" s="26">
+      <c r="D30" s="24">
         <v>0.4375</v>
       </c>
       <c r="E30" s="18">
@@ -1681,10 +1679,10 @@
       <c r="B31" s="18">
         <v>12</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C31" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D31" s="26">
+      <c r="D31" s="24">
         <v>0.4375</v>
       </c>
       <c r="E31" s="18">
@@ -1707,10 +1705,10 @@
       <c r="B32" s="18">
         <v>15</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C32" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D32" s="26">
+      <c r="D32" s="24">
         <v>0.4375</v>
       </c>
       <c r="E32" s="18">
@@ -1733,10 +1731,10 @@
       <c r="B33" s="18">
         <v>15</v>
       </c>
-      <c r="C33" s="26">
+      <c r="C33" s="24">
         <v>0.37847222222222227</v>
       </c>
-      <c r="D33" s="26">
+      <c r="D33" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E33" s="18">
@@ -1759,10 +1757,10 @@
       <c r="B34" s="18">
         <v>9</v>
       </c>
-      <c r="C34" s="26">
+      <c r="C34" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D34" s="26">
+      <c r="D34" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E34" s="18">
@@ -1785,10 +1783,10 @@
       <c r="B35" s="18">
         <v>21</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C35" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D35" s="26">
+      <c r="D35" s="24">
         <v>0.4375</v>
       </c>
       <c r="E35" s="18">
@@ -1811,10 +1809,10 @@
       <c r="B36" s="18">
         <v>1</v>
       </c>
-      <c r="C36" s="26">
+      <c r="C36" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D36" s="26">
+      <c r="D36" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E36" s="18">
@@ -1837,10 +1835,10 @@
       <c r="B37" s="18">
         <v>7</v>
       </c>
-      <c r="C37" s="26">
+      <c r="C37" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D37" s="26">
+      <c r="D37" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E37" s="18">
@@ -1863,10 +1861,10 @@
       <c r="B38" s="18">
         <v>19</v>
       </c>
-      <c r="C38" s="26">
+      <c r="C38" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D38" s="26">
+      <c r="D38" s="24">
         <v>0.4375</v>
       </c>
       <c r="E38" s="18">
@@ -1889,10 +1887,10 @@
       <c r="B39" s="18">
         <v>19</v>
       </c>
-      <c r="C39" s="26">
+      <c r="C39" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D39" s="26">
+      <c r="D39" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E39" s="18">
@@ -1915,10 +1913,10 @@
       <c r="B40" s="18">
         <v>6</v>
       </c>
-      <c r="C40" s="26">
+      <c r="C40" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D40" s="26">
+      <c r="D40" s="24">
         <v>0.70833333333333337</v>
       </c>
       <c r="E40" s="18">
@@ -1941,10 +1939,10 @@
       <c r="B41" s="18">
         <v>18</v>
       </c>
-      <c r="C41" s="26">
+      <c r="C41" s="24">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D41" s="26">
+      <c r="D41" s="24">
         <v>0.4375</v>
       </c>
       <c r="E41" s="18">
@@ -1991,553 +1989,553 @@
       <c r="C1" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="21">
-        <v>0</v>
-      </c>
-      <c r="B2" s="21" t="s">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2">
         <v>84107</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="21">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3">
         <v>84104</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="21">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4">
         <v>84106</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="21">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5">
         <v>84123</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="21">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6">
         <v>84115</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="21">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7">
         <v>84115</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="21">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8">
         <v>84104</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="21">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9">
         <v>84119</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="21">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10">
         <v>84103</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="21">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11">
         <v>84106</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="21">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12">
         <v>84118</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="21">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13">
         <v>84115</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="21">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14">
         <v>84103</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="21">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15">
         <v>84119</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="21">
+      <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16">
         <v>84119</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="21">
+      <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17">
         <v>84119</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.35">
-      <c r="A18" s="21">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D18" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18">
         <v>84119</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="21">
+      <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19">
         <v>84115</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="21">
+      <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20">
         <v>84115</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="21">
+      <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D21" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E21" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21">
         <v>84111</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="21">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D22" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="E22" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22">
         <v>84117</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="21">
+      <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="D23" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="E23" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="21">
+      <c r="F23">
         <v>84117</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="21">
+      <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="E24" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24">
         <v>84107</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="21">
+      <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D25" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25">
         <v>84118</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="21">
+      <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="21">
+      <c r="F26">
         <v>84117</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="21">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="21">
+      <c r="F27">
         <v>84105</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="21">
+      <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="21">
+      <c r="F28">
         <v>84121</v>
       </c>
     </row>
@@ -2555,8 +2553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AJ7" sqref="AJ7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE11" sqref="AE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4397,6 +4395,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39F2A75005F2D43B30369DAED2CCB1C" ma:contentTypeVersion="51" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dca2bb0f68bdf94cc5f80c9292ca56b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xmlns:ns3="1f707338-ea0f-4fe5-baee-59b996692b22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4cb8629785915e947a4406c57312ba8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4906,15 +4913,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC12B168-B9E1-4151-98F9-C97DA1AB8BBF}">
   <ds:schemaRefs/>
@@ -4922,6 +4920,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{346B5534-CC83-47DD-8523-BB97FB1B43B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4939,12 +4945,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
algorithm delivers multiple packages to same address now
</commit_message>
<xml_diff>
--- a/data/all_delivery_data.xlsx
+++ b/data/all_delivery_data.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamm\PycharmProjects\TravelingDeliveryman\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9F50E5-00A9-4F86-81DD-027CE31DC487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D869AC7-8791-47A8-8C0F-4DBA2151E24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4200" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="4200" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="package_data" sheetId="4" r:id="rId1"/>
-    <sheet name="address_data" sheetId="2" r:id="rId2"/>
-    <sheet name="distance_data" sheetId="1" r:id="rId3"/>
+    <sheet name="distance_data" sheetId="1" r:id="rId2"/>
+    <sheet name="address_data" sheetId="2" r:id="rId3"/>
     <sheet name="package_group_data" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">address_data!$A$1:$C$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2">address_data!$A$1:$C$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -880,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259C2A56-3C60-479F-941A-D591511CBD81}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1965,596 +1965,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4222C95-8038-46BE-A878-DD9F1771B676}">
-  <dimension ref="A1:F28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="19.08984375" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2">
-        <v>84107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3">
-        <v>84104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4">
-        <v>84106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5">
-        <v>84123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6">
-        <v>84115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7">
-        <v>84115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8">
-        <v>84104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9">
-        <v>84119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10">
-        <v>84103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11">
-        <v>84106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12">
-        <v>84118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13">
-        <v>84115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14">
-        <v>84103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15">
-        <v>84119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16">
-        <v>84119</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17">
-        <v>84119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18">
-        <v>84119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19">
-        <v>84115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20">
-        <v>84115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21">
-        <v>84111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22">
-        <v>84117</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23">
-        <v>84117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24">
-        <v>84107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25">
-        <v>84118</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26">
-        <v>84117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27">
-        <v>84105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28">
-        <v>84121</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:C28" xr:uid="{C4222C95-8038-46BE-A878-DD9F1771B676}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C28">
-      <sortCondition ref="A1:A28"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE11" sqref="AE11"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AG26" sqref="AG26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4272,6 +3688,591 @@
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4222C95-8038-46BE-A878-DD9F1771B676}">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="19.08984375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>84107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>84104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>84106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>84123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>84115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7">
+        <v>84115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8">
+        <v>84104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>84119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <v>84103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>84106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>84118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>84115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>84103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15">
+        <v>84119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16">
+        <v>84119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17">
+        <v>84119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18">
+        <v>84119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19">
+        <v>84115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20">
+        <v>84115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21">
+        <v>84111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22">
+        <v>84117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>84117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24">
+        <v>84107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25">
+        <v>84118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26">
+        <v>84117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27">
+        <v>84105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28">
+        <v>84121</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C28" xr:uid="{C4222C95-8038-46BE-A878-DD9F1771B676}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C28">
+      <sortCondition ref="A1:A28"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4395,15 +4396,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39F2A75005F2D43B30369DAED2CCB1C" ma:contentTypeVersion="51" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dca2bb0f68bdf94cc5f80c9292ca56b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xmlns:ns3="1f707338-ea0f-4fe5-baee-59b996692b22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4cb8629785915e947a4406c57312ba8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4913,6 +4905,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC12B168-B9E1-4151-98F9-C97DA1AB8BBF}">
   <ds:schemaRefs/>
@@ -4920,14 +4921,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{346B5534-CC83-47DD-8523-BB97FB1B43B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4945,4 +4938,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
can determine when is the earliest a truck can leave
</commit_message>
<xml_diff>
--- a/data/all_delivery_data.xlsx
+++ b/data/all_delivery_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamm\PycharmProjects\TravelingDeliveryman\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D869AC7-8791-47A8-8C0F-4DBA2151E24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{873131A2-CBCB-4FC7-847A-42D551E14E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4200" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="4200" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="package_data" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="75">
   <si>
     <t>address_id</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>location_name</t>
+  </si>
+  <si>
+    <t>address_available_time</t>
   </si>
 </sst>
 </file>
@@ -529,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -598,6 +601,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259C2A56-3C60-479F-941A-D591511CBD81}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -892,7 +899,7 @@
     <col min="7" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
@@ -917,8 +924,11 @@
       <c r="H1" s="22" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -943,8 +953,11 @@
       <c r="H2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -969,8 +982,11 @@
       <c r="H3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -995,8 +1011,11 @@
       <c r="H4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -1021,8 +1040,11 @@
       <c r="H5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -1047,8 +1069,11 @@
       <c r="H6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -1073,8 +1098,11 @@
       <c r="H7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -1099,8 +1127,11 @@
       <c r="H8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I8" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -1123,10 +1154,13 @@
         <v>0</v>
       </c>
       <c r="H9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="I9" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="18">
         <v>9</v>
       </c>
@@ -1134,7 +1168,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="24">
-        <v>0.43055555555555558</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D10" s="24">
         <v>0.70833333333333337</v>
@@ -1149,10 +1183,13 @@
         <v>0</v>
       </c>
       <c r="H10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="I10" s="27">
+        <v>0.43055555555555558</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="18">
         <v>10</v>
       </c>
@@ -1177,8 +1214,11 @@
       <c r="H11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I11" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="18">
         <v>11</v>
       </c>
@@ -1203,8 +1243,11 @@
       <c r="H12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I12" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="18">
         <v>12</v>
       </c>
@@ -1229,8 +1272,11 @@
       <c r="H13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I13" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="18">
         <v>13</v>
       </c>
@@ -1255,8 +1301,11 @@
       <c r="H14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I14" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="18">
         <v>14</v>
       </c>
@@ -1281,8 +1330,11 @@
       <c r="H15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I15" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="18">
         <v>15</v>
       </c>
@@ -1307,8 +1359,11 @@
       <c r="H16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="18">
         <v>16</v>
       </c>
@@ -1333,8 +1388,11 @@
       <c r="H17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="18">
         <v>17</v>
       </c>
@@ -1359,8 +1417,11 @@
       <c r="H18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="18">
         <v>18</v>
       </c>
@@ -1385,8 +1446,11 @@
       <c r="H19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I19" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="18">
         <v>19</v>
       </c>
@@ -1411,8 +1475,11 @@
       <c r="H20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="18">
         <v>20</v>
       </c>
@@ -1437,8 +1504,11 @@
       <c r="H21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="18">
         <v>21</v>
       </c>
@@ -1463,8 +1533,11 @@
       <c r="H22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I22" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="18">
         <v>22</v>
       </c>
@@ -1489,8 +1562,11 @@
       <c r="H23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I23" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="18">
         <v>23</v>
       </c>
@@ -1515,8 +1591,11 @@
       <c r="H24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="18">
         <v>24</v>
       </c>
@@ -1541,8 +1620,11 @@
       <c r="H25" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I25" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="18">
         <v>25</v>
       </c>
@@ -1567,8 +1649,11 @@
       <c r="H26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I26" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="18">
         <v>26</v>
       </c>
@@ -1593,8 +1678,11 @@
       <c r="H27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I27" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="18">
         <v>27</v>
       </c>
@@ -1619,8 +1707,11 @@
       <c r="H28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I28" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="18">
         <v>28</v>
       </c>
@@ -1645,8 +1736,11 @@
       <c r="H29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I29" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="18">
         <v>29</v>
       </c>
@@ -1671,8 +1765,11 @@
       <c r="H30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I30" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="18">
         <v>30</v>
       </c>
@@ -1697,8 +1794,11 @@
       <c r="H31" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I31" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="18">
         <v>31</v>
       </c>
@@ -1723,8 +1823,11 @@
       <c r="H32" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I32" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="18">
         <v>32</v>
       </c>
@@ -1749,8 +1852,11 @@
       <c r="H33" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I33" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="18">
         <v>33</v>
       </c>
@@ -1775,8 +1881,11 @@
       <c r="H34" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I34" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="18">
         <v>34</v>
       </c>
@@ -1801,8 +1910,11 @@
       <c r="H35" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I35" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="18">
         <v>35</v>
       </c>
@@ -1827,8 +1939,11 @@
       <c r="H36" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I36" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="18">
         <v>36</v>
       </c>
@@ -1853,8 +1968,11 @@
       <c r="H37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I37" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="18">
         <v>37</v>
       </c>
@@ -1879,8 +1997,11 @@
       <c r="H38" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I38" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="18">
         <v>38</v>
       </c>
@@ -1905,8 +2026,11 @@
       <c r="H39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I39" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="18">
         <v>39</v>
       </c>
@@ -1931,8 +2055,11 @@
       <c r="H40" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I40" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="18">
         <v>40</v>
       </c>
@@ -1955,6 +2082,9 @@
         <v>0</v>
       </c>
       <c r="H41" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" s="27">
         <v>0</v>
       </c>
     </row>
@@ -1968,7 +2098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AG26" sqref="AG26"/>
     </sheetView>
@@ -4396,6 +4526,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39F2A75005F2D43B30369DAED2CCB1C" ma:contentTypeVersion="51" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dca2bb0f68bdf94cc5f80c9292ca56b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xmlns:ns3="1f707338-ea0f-4fe5-baee-59b996692b22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4cb8629785915e947a4406c57312ba8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4905,15 +5044,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC12B168-B9E1-4151-98F9-C97DA1AB8BBF}">
   <ds:schemaRefs/>
@@ -4921,6 +5051,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{346B5534-CC83-47DD-8523-BB97FB1B43B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4938,12 +5076,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
all packages deliver on-time, does not yet account for package available time. all truck miles 222.0
</commit_message>
<xml_diff>
--- a/data/all_delivery_data.xlsx
+++ b/data/all_delivery_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamm\PycharmProjects\TravelingDeliveryman\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{873131A2-CBCB-4FC7-847A-42D551E14E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{293C7E9E-0F1E-42A2-81F1-3752E5BEC49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="4200" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -532,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -601,9 +601,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -888,7 +885,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -924,7 +921,7 @@
       <c r="H1" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="22" t="s">
         <v>74</v>
       </c>
     </row>
@@ -953,7 +950,7 @@
       <c r="H2" t="b">
         <v>0</v>
       </c>
-      <c r="I2" s="27">
+      <c r="I2" s="26">
         <v>0</v>
       </c>
     </row>
@@ -982,7 +979,7 @@
       <c r="H3" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="27">
+      <c r="I3" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1011,7 +1008,7 @@
       <c r="H4" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="27">
+      <c r="I4" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1040,7 +1037,7 @@
       <c r="H5" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="27">
+      <c r="I5" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1069,7 +1066,7 @@
       <c r="H6" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I6" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1098,7 +1095,7 @@
       <c r="H7" t="b">
         <v>0</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I7" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1127,7 +1124,7 @@
       <c r="H8" t="b">
         <v>0</v>
       </c>
-      <c r="I8" s="27">
+      <c r="I8" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1156,7 +1153,7 @@
       <c r="H9" t="b">
         <v>0</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I9" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1165,7 +1162,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="18">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C10" s="24">
         <v>0.33333333333333331</v>
@@ -1185,7 +1182,7 @@
       <c r="H10" t="b">
         <v>1</v>
       </c>
-      <c r="I10" s="27">
+      <c r="I10" s="26">
         <v>0.43055555555555558</v>
       </c>
     </row>
@@ -1214,7 +1211,7 @@
       <c r="H11" t="b">
         <v>0</v>
       </c>
-      <c r="I11" s="27">
+      <c r="I11" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1243,7 +1240,7 @@
       <c r="H12" t="b">
         <v>0</v>
       </c>
-      <c r="I12" s="27">
+      <c r="I12" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1272,7 +1269,7 @@
       <c r="H13" t="b">
         <v>0</v>
       </c>
-      <c r="I13" s="27">
+      <c r="I13" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1301,7 +1298,7 @@
       <c r="H14" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="27">
+      <c r="I14" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1330,7 +1327,7 @@
       <c r="H15" t="b">
         <v>0</v>
       </c>
-      <c r="I15" s="27">
+      <c r="I15" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1359,7 +1356,7 @@
       <c r="H16" t="b">
         <v>0</v>
       </c>
-      <c r="I16" s="27">
+      <c r="I16" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1388,7 +1385,7 @@
       <c r="H17" t="b">
         <v>0</v>
       </c>
-      <c r="I17" s="27">
+      <c r="I17" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1417,7 +1414,7 @@
       <c r="H18" t="b">
         <v>0</v>
       </c>
-      <c r="I18" s="27">
+      <c r="I18" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1446,7 +1443,7 @@
       <c r="H19" t="b">
         <v>0</v>
       </c>
-      <c r="I19" s="27">
+      <c r="I19" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1475,7 +1472,7 @@
       <c r="H20" t="b">
         <v>0</v>
       </c>
-      <c r="I20" s="27">
+      <c r="I20" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1504,7 +1501,7 @@
       <c r="H21" t="b">
         <v>0</v>
       </c>
-      <c r="I21" s="27">
+      <c r="I21" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1533,7 +1530,7 @@
       <c r="H22" t="b">
         <v>0</v>
       </c>
-      <c r="I22" s="27">
+      <c r="I22" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1562,7 +1559,7 @@
       <c r="H23" t="b">
         <v>0</v>
       </c>
-      <c r="I23" s="27">
+      <c r="I23" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1591,7 +1588,7 @@
       <c r="H24" t="b">
         <v>0</v>
       </c>
-      <c r="I24" s="27">
+      <c r="I24" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1620,7 +1617,7 @@
       <c r="H25" t="b">
         <v>0</v>
       </c>
-      <c r="I25" s="27">
+      <c r="I25" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1649,7 +1646,7 @@
       <c r="H26" t="b">
         <v>0</v>
       </c>
-      <c r="I26" s="27">
+      <c r="I26" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1678,7 +1675,7 @@
       <c r="H27" t="b">
         <v>0</v>
       </c>
-      <c r="I27" s="27">
+      <c r="I27" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1707,7 +1704,7 @@
       <c r="H28" t="b">
         <v>0</v>
       </c>
-      <c r="I28" s="27">
+      <c r="I28" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1736,7 +1733,7 @@
       <c r="H29" t="b">
         <v>0</v>
       </c>
-      <c r="I29" s="27">
+      <c r="I29" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1765,7 +1762,7 @@
       <c r="H30" t="b">
         <v>0</v>
       </c>
-      <c r="I30" s="27">
+      <c r="I30" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1794,7 +1791,7 @@
       <c r="H31" t="b">
         <v>0</v>
       </c>
-      <c r="I31" s="27">
+      <c r="I31" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1823,7 +1820,7 @@
       <c r="H32" t="b">
         <v>0</v>
       </c>
-      <c r="I32" s="27">
+      <c r="I32" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1852,7 +1849,7 @@
       <c r="H33" t="b">
         <v>0</v>
       </c>
-      <c r="I33" s="27">
+      <c r="I33" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1881,7 +1878,7 @@
       <c r="H34" t="b">
         <v>0</v>
       </c>
-      <c r="I34" s="27">
+      <c r="I34" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1910,7 +1907,7 @@
       <c r="H35" t="b">
         <v>0</v>
       </c>
-      <c r="I35" s="27">
+      <c r="I35" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1939,7 +1936,7 @@
       <c r="H36" t="b">
         <v>0</v>
       </c>
-      <c r="I36" s="27">
+      <c r="I36" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1968,7 +1965,7 @@
       <c r="H37" t="b">
         <v>0</v>
       </c>
-      <c r="I37" s="27">
+      <c r="I37" s="26">
         <v>0</v>
       </c>
     </row>
@@ -1997,7 +1994,7 @@
       <c r="H38" t="b">
         <v>0</v>
       </c>
-      <c r="I38" s="27">
+      <c r="I38" s="26">
         <v>0</v>
       </c>
     </row>
@@ -2026,7 +2023,7 @@
       <c r="H39" t="b">
         <v>0</v>
       </c>
-      <c r="I39" s="27">
+      <c r="I39" s="26">
         <v>0</v>
       </c>
     </row>
@@ -2055,7 +2052,7 @@
       <c r="H40" t="b">
         <v>0</v>
       </c>
-      <c r="I40" s="27">
+      <c r="I40" s="26">
         <v>0</v>
       </c>
     </row>
@@ -2084,7 +2081,7 @@
       <c r="H41" t="b">
         <v>0</v>
       </c>
-      <c r="I41" s="27">
+      <c r="I41" s="26">
         <v>0</v>
       </c>
     </row>
@@ -2099,8 +2096,8 @@
   <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG26" sqref="AG26"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3825,7 +3822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4222C95-8038-46BE-A878-DD9F1771B676}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -4526,15 +4523,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39F2A75005F2D43B30369DAED2CCB1C" ma:contentTypeVersion="51" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dca2bb0f68bdf94cc5f80c9292ca56b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xmlns:ns3="1f707338-ea0f-4fe5-baee-59b996692b22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4cb8629785915e947a4406c57312ba8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5044,6 +5032,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC12B168-B9E1-4151-98F9-C97DA1AB8BBF}">
   <ds:schemaRefs/>
@@ -5051,14 +5048,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{346B5534-CC83-47DD-8523-BB97FB1B43B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5076,4 +5065,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>